<commit_message>
update rules & process ot lieu
</commit_message>
<xml_diff>
--- a/uploads/rules.xlsx
+++ b/uploads/rules.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,11 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>